<commit_message>
see similarityStatus.xlsx for insertion methods, somewhat working for unbounded tree width, need to check supers' overlap
</commit_message>
<xml_diff>
--- a/similarityStatus.xlsx
+++ b/similarityStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataCopied\Research\tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549E92E8-7667-4804-8FB9-11EE6A6F2102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6C4A02-D1DF-4189-AA09-DB804633134A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{442E57C3-00D2-4243-884C-C4C66AC44C45}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12370" windowHeight="10200" xr2:uid="{442E57C3-00D2-4243-884C-C4C66AC44C45}"/>
   </bookViews>
   <sheets>
     <sheet name="SimilarityStatus" sheetId="1" r:id="rId1"/>
@@ -131,9 +131,6 @@
     <t>create new branch and insert seq to ambi</t>
   </si>
   <si>
-    <t>insert seq to ambi</t>
-  </si>
-  <si>
     <t>4 a) only 1 branch</t>
   </si>
   <si>
@@ -152,19 +149,22 @@
     <t>create super then traverse again with the closest one. May want to to rotation or promotion</t>
   </si>
   <si>
-    <t>do like method 6 or 8 then see if the new t_parent stay with any of the super (it should be) then if the child is closer to t_parent, create super for once then move the child there. Update all above</t>
-  </si>
-  <si>
     <t>4 and 5</t>
   </si>
   <si>
-    <t>do like method 7 or 8 then see if the new t_parent stay with any of the super (it should be) then if the child is closer to t_parent, create super for once then move the child there. Update all above</t>
-  </si>
-  <si>
     <t>2 and 4 and 5</t>
   </si>
   <si>
-    <t>do like method 8 then see if the new t_parent stay with any of the super (it should be) then if the child is closer to t_parent, create super for once then move the child there. Update all above</t>
+    <t>do like method 5 or 7 then see if the new t_parent stay with any of the super (it should be) then if the child is closer to t_parent, create super for once then move the child there. Update all above</t>
+  </si>
+  <si>
+    <t>do like method 6 or 7 then see if the new t_parent stay with any of the super (it should be) then if the child is closer to t_parent, create super for once then move the child there. Update all above</t>
+  </si>
+  <si>
+    <t>do like method 7 then see if the new t_parent stay with any of the super (it should be) then if the child is closer to t_parent, create super for once then move the child there. Update all above</t>
+  </si>
+  <si>
+    <t>If the branch has more than 3 children (aka &gt;2 leaves + 1 ambi), check if seq stay with any leave. Else, insert seq to ambi (create 1 if hasn't). Then, if the priority of ambi &gt;= stay threshold, make this ambi node non-ambi.</t>
   </si>
 </sst>
 </file>
@@ -276,13 +276,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62626FA3-E153-43EE-8DA8-5F5B5E84444A}" name="methods" displayName="methods" ref="A13:D24" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62626FA3-E153-43EE-8DA8-5F5B5E84444A}" name="methods" displayName="methods" ref="A13:D24" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A13:D24" xr:uid="{62626FA3-E153-43EE-8DA8-5F5B5E84444A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CE5325F3-9EF6-48F1-B0B4-5A6994764319}" name="method" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{746EA876-C065-4C3F-9DA1-F0AAAB0EA48F}" name="condition combo" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{FDE30575-D299-4965-84EC-878E663866EB}" name="algo" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{0A239C60-7C31-4F8B-A859-861120D71879}" name="remarks" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CE5325F3-9EF6-48F1-B0B4-5A6994764319}" name="method" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{746EA876-C065-4C3F-9DA1-F0AAAB0EA48F}" name="condition combo" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FDE30575-D299-4965-84EC-878E663866EB}" name="algo" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{0A239C60-7C31-4F8B-A859-861120D71879}" name="remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0D6BE0-7CF6-4D75-A762-F9BAED9E324E}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -790,10 +790,10 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -808,15 +808,15 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -825,10 +825,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -837,10 +837,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D22" s="2"/>
     </row>
@@ -849,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>40</v>
@@ -861,10 +861,10 @@
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D24" s="2"/>
     </row>

</xml_diff>

<commit_message>
fixed bug for add subtree, changed foundation, need test
</commit_message>
<xml_diff>
--- a/similarityStatus.xlsx
+++ b/similarityStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataCopied\Research\tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6C4A02-D1DF-4189-AA09-DB804633134A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85D1FDB-7E70-4113-B98C-5313FFE799C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12370" windowHeight="10200" xr2:uid="{442E57C3-00D2-4243-884C-C4C66AC44C45}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{442E57C3-00D2-4243-884C-C4C66AC44C45}"/>
   </bookViews>
   <sheets>
     <sheet name="SimilarityStatus" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>leaf</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>If the branch has more than 3 children (aka &gt;2 leaves + 1 ambi), check if seq stay with any leave. Else, insert seq to ambi (create 1 if hasn't). Then, if the priority of ambi &gt;= stay threshold, make this ambi node non-ambi.</t>
+  </si>
+  <si>
+    <t>root</t>
   </si>
 </sst>
 </file>
@@ -250,8 +253,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31B97322-E66D-4B74-B18C-2039BFBF058A}" name="Conditions" displayName="Conditions" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{31B97322-E66D-4B74-B18C-2039BFBF058A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31B97322-E66D-4B74-B18C-2039BFBF058A}" name="Conditions" displayName="Conditions" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{31B97322-E66D-4B74-B18C-2039BFBF058A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A6D084B0-AC1D-408B-8E30-910F8023A935}" name="Node Type"/>
     <tableColumn id="2" xr3:uid="{D5A1AAB6-AF87-4D3C-8429-00424CF6E2DC}" name="stay"/>
@@ -263,8 +266,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{233A0315-22C8-42B9-A23D-EFA529E19AF0}" name="ConditionCodes" displayName="ConditionCodes" ref="A8:D11" totalsRowShown="0">
-  <autoFilter ref="A8:D11" xr:uid="{233A0315-22C8-42B9-A23D-EFA529E19AF0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{233A0315-22C8-42B9-A23D-EFA529E19AF0}" name="ConditionCodes" displayName="ConditionCodes" ref="A9:D13" totalsRowShown="0">
+  <autoFilter ref="A9:D13" xr:uid="{233A0315-22C8-42B9-A23D-EFA529E19AF0}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C4D9B5C4-A82E-4C06-A487-F0E004993E05}" name="Node Type"/>
     <tableColumn id="2" xr3:uid="{651DBF82-2602-42E2-84CE-49C6F253CA88}" name="stay"/>
@@ -276,8 +279,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62626FA3-E153-43EE-8DA8-5F5B5E84444A}" name="methods" displayName="methods" ref="A13:D24" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A13:D24" xr:uid="{62626FA3-E153-43EE-8DA8-5F5B5E84444A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62626FA3-E153-43EE-8DA8-5F5B5E84444A}" name="methods" displayName="methods" ref="A15:D26" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A15:D26" xr:uid="{62626FA3-E153-43EE-8DA8-5F5B5E84444A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CE5325F3-9EF6-48F1-B0B4-5A6994764319}" name="method" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{746EA876-C065-4C3F-9DA1-F0AAAB0EA48F}" name="condition combo" dataDxfId="2"/>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0D6BE0-7CF6-4D75-A762-F9BAED9E324E}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,216 +660,244 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
         <v>1</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>3</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" ht="174" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="145" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
-        <v>6</v>
+    <row r="20" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
         <v>7</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
         <v>8</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
         <v>9</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
         <v>10</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>